<commit_message>
Update RQ file, searh terms
</commit_message>
<xml_diff>
--- a/gradu/seachterms.xlsx
+++ b/gradu/seachterms.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Yliopisto\gradu\aigrad\gradu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF59E838-1029-4E29-A0B0-08F6AF2A85F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97095AA4-33EB-45A9-85C2-3815B9D18C98}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{510022EC-A773-469C-9D8E-0E75BD5962EC}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Search terms and databases</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Good articles, many came from AGI journal</t>
   </si>
   <si>
-    <t>Should journals be looked through manually? AI, AGI, AIR</t>
-  </si>
-  <si>
     <t>scidi</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>limited to research/review/conference papers. Too many chemistry related papers.</t>
   </si>
   <si>
-    <t>AGIS and other irrelevant terms mess up searches. Chemistry papers also show up sometimes even though search is limited to papers relating to AI</t>
-  </si>
-  <si>
     <t>(agi OR "artificial general intelligence" OR "general artificial intelligence") AND (ai OR "artificial intelligence" OR computer)</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t xml:space="preserve">102 of which were book chapters. </t>
   </si>
   <si>
-    <t>gs doesn't show the results' types, thus lots of manual work if no books are involved.</t>
-  </si>
-  <si>
     <t>"strong ai" AND (agi OR "artificial general intelligence" OR "general artificial intelligence")</t>
   </si>
   <si>
@@ -144,13 +135,52 @@
   </si>
   <si>
     <t>43 of which were book chapters.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ("artificial intelligence" AND ("general intelligence" OR "artificial general intelligence"))</t>
+  </si>
+  <si>
+    <t>Focused and produces relevant papers</t>
+  </si>
+  <si>
+    <t>Too many natural science articles</t>
+  </si>
+  <si>
+    <t>Should journals be looked through manually? AI, AGI, AIR + conference papers</t>
+  </si>
+  <si>
+    <t>Good results in multiple search engines.</t>
+  </si>
+  <si>
+    <t>Bad or few results.</t>
+  </si>
+  <si>
+    <t>Good results, but only in few SEs.</t>
+  </si>
+  <si>
+    <t>Also irrelevant papers</t>
+  </si>
+  <si>
+    <t>Seems ok, but too many papers to handle</t>
+  </si>
+  <si>
+    <t>Plenty of results, maybe even too much. Needs tweaking.</t>
+  </si>
+  <si>
+    <t>Search phrase ranking</t>
+  </si>
+  <si>
+    <t>GS doesn't show the results' types, thus lots of manual work if books, notes, and other bad sources are to be excluded.</t>
+  </si>
+  <si>
+    <t>AGIS and other irrelevant terms mess up searches. Natural science papers also show up sometimes even though search is limited to papers relating to AI.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,8 +203,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -222,8 +273,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -231,13 +297,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1"/>
@@ -248,9 +332,17 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="5"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Aksentti6" xfId="5" builtinId="49"/>
+    <cellStyle name="Huono" xfId="3" builtinId="27"/>
     <cellStyle name="Hyvä" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutraali" xfId="4" builtinId="28"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
     <cellStyle name="Selittävä teksti" xfId="2" builtinId="53"/>
   </cellStyles>
@@ -564,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C9067E-67BE-4864-9AD9-5D5C69A2FCBF}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,254 +676,349 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
+      <c r="E1" s="10" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>37</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>45</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E5" s="13" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="3">
-        <v>21300</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
       <c r="D9" s="3">
+        <v>21300</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="3">
         <v>16700</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D12" s="3">
         <v>113</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D13" s="3">
         <v>200</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E13" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D14" s="3">
         <v>810</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3">
         <v>3077</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="B17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="3">
+        <v>585</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3">
+        <v>707</v>
+      </c>
+      <c r="E18" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14" s="3">
-        <v>585</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="7" t="s">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="3">
+        <v>6010</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="3">
+        <v>2820</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="3">
+        <v>3897</v>
+      </c>
+      <c r="E23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="3">
-        <v>707</v>
-      </c>
-      <c r="E15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="5" t="s">
+      <c r="D24" s="3">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D25" s="3">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="3">
-        <v>6010</v>
-      </c>
-      <c r="E18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="3">
-        <v>2820</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="3">
+      <c r="D27" s="3">
         <v>784</v>
-      </c>
-      <c r="E20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="3">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" s="3">
-        <v>0</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="3">
-        <v>2</v>
-      </c>
-      <c r="E23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="3">
-        <v>63</v>
-      </c>
-      <c r="E24" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3">
-        <v>2170</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27">
-        <v>138</v>
       </c>
       <c r="E27" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31" s="3">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="3">
+        <v>1407</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D34">
+        <v>138</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D35" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37">
+        <v>59</v>
+      </c>
+      <c r="E37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38">
+        <v>76</v>
+      </c>
+      <c r="E38" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="3">
+        <v>6150</v>
+      </c>
+      <c r="E39" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add scopus material to sheet
</commit_message>
<xml_diff>
--- a/gradu/seachterms.xlsx
+++ b/gradu/seachterms.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="73">
   <si>
     <t xml:space="preserve">Search terms and databases</t>
   </si>
@@ -233,15 +233,22 @@
   </si>
   <si>
     <t xml:space="preserve">Total hits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potential</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accepted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -452,7 +459,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -475,8 +482,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="29">
+  <cellStyleXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -527,8 +541,14 @@
     <xf numFmtId="164" fontId="11" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -633,8 +653,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="29" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="30" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
@@ -650,6 +682,8 @@
     <cellStyle name="Excel Built-in Neutral" xfId="26"/>
     <cellStyle name="Excel Built-in Bad" xfId="27"/>
     <cellStyle name="Excel Built-in Accent6" xfId="28"/>
+    <cellStyle name="Accent 1" xfId="29"/>
+    <cellStyle name="Accent 2" xfId="30"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -719,10 +753,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R55"/>
+  <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G50" activeCellId="0" sqref="G50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1256,6 +1290,12 @@
       <c r="G50" s="17" t="s">
         <v>70</v>
       </c>
+      <c r="H50" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I50" s="27" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="19" t="s">
@@ -1295,6 +1335,12 @@
       </c>
       <c r="G55" s="0" t="n">
         <v>12</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G56" s="28" t="n">
+        <f aca="false">SUM(G51:G55)</f>
+        <v>191</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add JAGI papers to sheet
</commit_message>
<xml_diff>
--- a/gradu/seachterms.xlsx
+++ b/gradu/seachterms.xlsx
@@ -250,7 +250,7 @@
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -330,8 +330,15 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,7 +348,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
+        <bgColor rgb="FF000080"/>
       </patternFill>
     </fill>
     <fill>
@@ -359,7 +366,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FFC5E0B4"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -382,6 +389,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC5E0B4"/>
         <bgColor rgb="FFC6EFCE"/>
       </patternFill>
@@ -430,32 +443,32 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2A6099"/>
+        <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF9C0006"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF8000"/>
+        <bgColor rgb="FFFF8080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF00A933"/>
         <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF2A6099"/>
-        <bgColor rgb="FF4472C4"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FF9C0006"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF8000"/>
-        <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
@@ -490,7 +503,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -517,9 +530,15 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
@@ -541,47 +560,44 @@
     <xf numFmtId="164" fontId="11" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="26" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="27" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="1" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="26" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="27" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="0" xfId="28" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="7" borderId="0" xfId="29" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="1" xfId="30" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="10" borderId="0" xfId="27" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="0" xfId="30" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -589,10 +605,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -605,27 +617,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="16" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="17" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="17" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="31" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -649,15 +665,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="23" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="29" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="30" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="25" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="22" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="0" xfId="31" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -666,24 +690,25 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="18">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Accent 1 3" xfId="20"/>
-    <cellStyle name="Accent 2 2" xfId="21"/>
-    <cellStyle name="Heading 1 1" xfId="22"/>
-    <cellStyle name="Neutral 4" xfId="23"/>
-    <cellStyle name="Excel Built-in Good" xfId="24"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="25"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="26"/>
-    <cellStyle name="Excel Built-in Bad" xfId="27"/>
-    <cellStyle name="Excel Built-in Accent6" xfId="28"/>
-    <cellStyle name="Accent 1" xfId="29"/>
-    <cellStyle name="Accent 2" xfId="30"/>
+    <cellStyle name="Accent 1 1" xfId="20"/>
+    <cellStyle name="Accent 1 3" xfId="21"/>
+    <cellStyle name="Accent 2 2" xfId="22"/>
+    <cellStyle name="Accent 2 3" xfId="23"/>
+    <cellStyle name="Heading 1 1" xfId="24"/>
+    <cellStyle name="Neutral 4" xfId="25"/>
+    <cellStyle name="Excel Built-in Good" xfId="26"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="27"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="28"/>
+    <cellStyle name="Excel Built-in Bad" xfId="29"/>
+    <cellStyle name="Excel Built-in Accent6" xfId="30"/>
+    <cellStyle name="Good" xfId="31"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -696,7 +721,7 @@
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF9C0006"/>
-      <rgbColor rgb="FF006100"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
@@ -706,7 +731,7 @@
       <rgbColor rgb="FF8FAADC"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFFFD7D7"/>
+      <rgbColor rgb="FFC6EFCE"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF2A6099"/>
@@ -720,8 +745,8 @@
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFC6EFCE"/>
+      <rgbColor rgb="FFFFD7D7"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFEB9C"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -737,7 +762,7 @@
       <rgbColor rgb="FF7F7F7F"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF548235"/>
-      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF006100"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF9C5700"/>
       <rgbColor rgb="FF993366"/>
@@ -755,7 +780,7 @@
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H52" activeCellId="0" sqref="H52"/>
     </sheetView>
   </sheetViews>
@@ -1298,7 +1323,7 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="19" t="s">
+      <c r="B51" s="28" t="s">
         <v>52</v>
       </c>
       <c r="G51" s="0" t="n">
@@ -1309,7 +1334,7 @@
       <c r="B52" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="G52" s="0" t="n">
+      <c r="G52" s="29" t="n">
         <v>3</v>
       </c>
     </row>
@@ -1317,7 +1342,7 @@
       <c r="B53" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="G53" s="0" t="n">
+      <c r="G53" s="29" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1333,12 +1358,12 @@
       <c r="B55" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="G55" s="0" t="n">
+      <c r="G55" s="29" t="n">
         <v>12</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G56" s="28" t="n">
+      <c r="G56" s="30" t="n">
         <f aca="false">SUM(G51:G55)</f>
         <v>191</v>
       </c>

</xml_diff>